<commit_message>
Updates with major refactoring of footings framework.
</commit_message>
<xml_diff>
--- a/tests/core/data/expected-footings-wb.xlsx
+++ b/tests/core/data/expected-footings-wb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="test-builtins" sheetId="1" state="visible" r:id="rId2"/>
@@ -77,7 +77,7 @@
     <t xml:space="preserve">('tuple', 'key')</t>
   </si>
   <si>
-    <t xml:space="preserve">callable: core.test_xlsx.test_footings_xlsx_wb.&lt;locals&gt;.test_func</t>
+    <t xml:space="preserve">callable: test_xlsx.test_footings_xlsx_wb.&lt;locals&gt;.test_func</t>
   </si>
   <si>
     <t xml:space="preserve">worksheet</t>
@@ -250,11 +250,11 @@
   </sheetPr>
   <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.44"/>
@@ -701,13 +701,13 @@
   </sheetPr>
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>

</xml_diff>